<commit_message>
Tickets Chart update with the last days
</commit_message>
<xml_diff>
--- a/Documents/Tickets Chart - Duck Squad.xlsx
+++ b/Documents/Tickets Chart - Duck Squad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inesc\Desktop\Projetos Git\Sprint3\DuckSoftWorks\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2558ED13-6433-4694-B991-8B3E45D7B224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDCD78A-76F0-4395-8407-CC8E8A31BD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="117">
   <si>
     <t>Week 1</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>Frontend corrections</t>
+  </si>
+  <si>
+    <t>PDS avaluation</t>
+  </si>
+  <si>
+    <t>POOJ avaluation</t>
+  </si>
+  <si>
+    <t>Client presentation</t>
   </si>
 </sst>
 </file>
@@ -1482,16 +1491,26 @@
     <xf numFmtId="0" fontId="11" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1500,87 +1519,22 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="173">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF548135"/>
-          <bgColor rgb="FF548135"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF88D608"/>
-          <bgColor rgb="FF88D608"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1F3864"/>
-          <bgColor rgb="FF1F3864"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF2C073B"/>
-          <bgColor rgb="FF2C073B"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="168">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2903,6 +2857,61 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF548135"/>
+          <bgColor rgb="FF548135"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF88D608"/>
+          <bgColor rgb="FF88D608"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF1F3864"/>
+          <bgColor rgb="FF1F3864"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF2C073B"/>
+          <bgColor rgb="FF2C073B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFF2F2F2"/>
       </font>
       <fill>
@@ -2975,61 +2984,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF7F7F7F"/>
           <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF548135"/>
-          <bgColor rgb="FF548135"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF88D608"/>
-          <bgColor rgb="FF88D608"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1F3864"/>
-          <bgColor rgb="FF1F3864"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF590F77"/>
-          <bgColor rgb="FF590F77"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3667,17 +3621,17 @@
         <v>0</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="117"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="123"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1">
       <c r="F3" s="2"/>
@@ -3709,11 +3663,11 @@
       <c r="P4" s="10"/>
     </row>
     <row r="5" spans="2:19">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="3">
@@ -3727,10 +3681,10 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="10"/>
-      <c r="R5" s="131" t="s">
+      <c r="R5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="131"/>
+      <c r="S5" s="117"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="11" t="s">
@@ -3739,7 +3693,7 @@
       <c r="C6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="119"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="3">
@@ -3764,10 +3718,10 @@
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="114"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -3793,10 +3747,10 @@
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="114"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -3822,10 +3776,10 @@
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -3851,10 +3805,10 @@
       <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -3880,10 +3834,10 @@
       <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -3903,10 +3857,10 @@
       <c r="B12" s="11">
         <v>12</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -5075,138 +5029,138 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="H2:P2"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="containsText" dxfId="172" priority="1" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="167" priority="1" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="171" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="170" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="169" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="168" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="163" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="167" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="6" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="166" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="7" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="165" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="8" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="164" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="9" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="163" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="10" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="162" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="11" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="161" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="12" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="160" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="21" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="159" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="22" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="158" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="23" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="157" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="24" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="156" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="25" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="containsText" dxfId="155" priority="26" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="150" priority="26" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(B6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="154" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="27" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="153" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="152" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="151" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="30" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="150" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="31" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="149" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="32" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5245,17 +5199,17 @@
         <v>31</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="117"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="123"/>
     </row>
     <row r="3" spans="2:20" ht="15" customHeight="1">
       <c r="F3" s="2"/>
@@ -5349,11 +5303,11 @@
       <c r="P8" s="34"/>
     </row>
     <row r="9" spans="2:20">
-      <c r="B9" s="131" t="s">
+      <c r="B9" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
       <c r="E9" s="20"/>
       <c r="F9" s="21" t="s">
         <v>32</v>
@@ -5372,10 +5326,10 @@
       <c r="N9" s="8"/>
       <c r="O9" s="35"/>
       <c r="P9" s="34"/>
-      <c r="S9" s="131" t="s">
+      <c r="S9" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="T9" s="131"/>
+      <c r="T9" s="117"/>
     </row>
     <row r="10" spans="2:20">
       <c r="B10" s="11" t="s">
@@ -5384,7 +5338,7 @@
       <c r="C10" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21" t="s">
         <v>33</v>
@@ -5416,10 +5370,10 @@
       <c r="B11" s="11">
         <v>1</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="20"/>
       <c r="F11" s="25" t="s">
         <v>34</v>
@@ -5454,10 +5408,10 @@
       <c r="B12" s="11">
         <v>2</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="20"/>
       <c r="F12" s="25" t="s">
         <v>35</v>
@@ -5489,10 +5443,10 @@
       <c r="B13" s="11">
         <v>3</v>
       </c>
-      <c r="C13" s="113" t="s">
+      <c r="C13" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="114"/>
+      <c r="D13" s="119"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25" t="s">
         <v>6</v>
@@ -5524,10 +5478,10 @@
       <c r="B14" s="11">
         <v>5</v>
       </c>
-      <c r="C14" s="113" t="s">
+      <c r="C14" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="114"/>
+      <c r="D14" s="119"/>
       <c r="E14" s="20"/>
       <c r="F14" s="25" t="s">
         <v>36</v>
@@ -5559,10 +5513,10 @@
       <c r="B15" s="11">
         <v>8</v>
       </c>
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="114"/>
+      <c r="D15" s="119"/>
       <c r="E15" s="20"/>
       <c r="F15" s="25" t="s">
         <v>37</v>
@@ -5588,10 +5542,10 @@
       <c r="B16" s="11">
         <v>12</v>
       </c>
-      <c r="C16" s="113" t="s">
+      <c r="C16" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="114"/>
+      <c r="D16" s="119"/>
       <c r="E16" s="20"/>
       <c r="F16" s="25" t="s">
         <v>38</v>
@@ -6708,76 +6662,76 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="H2:P2"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="containsText" dxfId="148" priority="6" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="143" priority="6" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="147" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="7" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="146" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="145" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="144" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="10" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="143" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="11" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G22">
-    <cfRule type="cellIs" dxfId="142" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="12" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="141" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="13" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="140" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="14" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="139" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="15" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="138" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="16" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="137" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="17" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6819,27 +6773,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="1" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="2" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="3" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="4" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="5" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6883,17 +6837,17 @@
         <v>0</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="117"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="123"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1">
       <c r="F3" s="2"/>
@@ -6929,11 +6883,11 @@
       <c r="P4" s="34"/>
     </row>
     <row r="5" spans="2:19">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
       <c r="F5" s="21" t="s">
         <v>41</v>
       </c>
@@ -6951,10 +6905,10 @@
       <c r="N5" s="27"/>
       <c r="O5" s="27"/>
       <c r="P5" s="34"/>
-      <c r="R5" s="131" t="s">
+      <c r="R5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="131"/>
+      <c r="S5" s="117"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="11" t="s">
@@ -6963,7 +6917,7 @@
       <c r="C6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="119"/>
       <c r="F6" s="25" t="s">
         <v>42</v>
       </c>
@@ -6992,10 +6946,10 @@
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="114"/>
+      <c r="D7" s="119"/>
       <c r="F7" s="25" t="s">
         <v>43</v>
       </c>
@@ -7024,10 +6978,10 @@
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="114"/>
+      <c r="D8" s="119"/>
       <c r="F8" s="25" t="s">
         <v>44</v>
       </c>
@@ -7056,10 +7010,10 @@
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="119"/>
       <c r="F9" s="25" t="s">
         <v>45</v>
       </c>
@@ -7088,10 +7042,10 @@
       <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="F10" s="25" t="s">
         <v>46</v>
       </c>
@@ -7120,10 +7074,10 @@
       <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="F11" s="25" t="s">
         <v>47</v>
       </c>
@@ -7146,10 +7100,10 @@
       <c r="B12" s="11">
         <v>12</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="119"/>
       <c r="F12" s="25" t="s">
         <v>48</v>
       </c>
@@ -8326,138 +8280,138 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="H2:P2"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="containsText" dxfId="124" priority="1" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="cellIs" dxfId="123" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="cellIs" dxfId="122" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="cellIs" dxfId="121" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="cellIs" dxfId="120" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="115" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="cellIs" dxfId="119" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="114" priority="6" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="cellIs" dxfId="118" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="7" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="containsText" dxfId="117" priority="8" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(B6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="116" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="9" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="115" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="114" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="113" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="108" priority="12" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="112" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="107" priority="13" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="111" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="14" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="110" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="16" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="109" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="17" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="108" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="18" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="107" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="19" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P20">
-    <cfRule type="cellIs" dxfId="106" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="20" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="105" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="29" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="104" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="30" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="103" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="31" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="102" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="32" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="101" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="33" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8505,24 +8459,24 @@
         <v>31</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="117"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="123"/>
     </row>
     <row r="4" spans="2:20" ht="16.5" customHeight="1">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
       <c r="F4" s="61" t="s">
         <v>58</v>
       </c>
@@ -8543,10 +8497,10 @@
         <v>6</v>
       </c>
       <c r="Q4" s="10"/>
-      <c r="S4" s="131" t="s">
+      <c r="S4" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="131"/>
+      <c r="T4" s="117"/>
     </row>
     <row r="5" spans="2:20" ht="16.5" customHeight="1">
       <c r="B5" s="11" t="s">
@@ -8555,7 +8509,7 @@
       <c r="C5" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="114"/>
+      <c r="D5" s="119"/>
       <c r="F5" s="61" t="s">
         <v>59</v>
       </c>
@@ -8587,10 +8541,10 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="113" t="s">
+      <c r="C6" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="119"/>
       <c r="F6" s="61" t="s">
         <v>60</v>
       </c>
@@ -8622,10 +8576,10 @@
       <c r="B7" s="11">
         <v>2</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="114"/>
+      <c r="D7" s="119"/>
       <c r="F7" s="61" t="s">
         <v>61</v>
       </c>
@@ -8657,10 +8611,10 @@
       <c r="B8" s="11">
         <v>3</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="114"/>
+      <c r="D8" s="119"/>
       <c r="F8" s="66" t="s">
         <v>62</v>
       </c>
@@ -8692,10 +8646,10 @@
       <c r="B9" s="11">
         <v>5</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="119"/>
       <c r="F9" s="66" t="s">
         <v>63</v>
       </c>
@@ -8729,10 +8683,10 @@
       <c r="B10" s="11">
         <v>8</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="F10" s="66" t="s">
         <v>64</v>
       </c>
@@ -8758,10 +8712,10 @@
       <c r="B11" s="11">
         <v>12</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="F11" s="66" t="s">
         <v>34</v>
       </c>
@@ -12296,138 +12250,138 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="containsText" dxfId="100" priority="1" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="cellIs" dxfId="99" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="cellIs" dxfId="98" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="cellIs" dxfId="97" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="cellIs" dxfId="96" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="91" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="cellIs" dxfId="95" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="6" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G1001">
-    <cfRule type="cellIs" dxfId="94" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="7" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P38 Q9 Q12 Q23">
-    <cfRule type="cellIs" dxfId="93" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="8" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P38 Q9 Q12 Q23">
-    <cfRule type="cellIs" dxfId="92" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="9" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P38 Q9 Q12 Q23">
-    <cfRule type="cellIs" dxfId="91" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="10" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P38 Q9 Q12 Q23">
-    <cfRule type="cellIs" dxfId="90" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="11" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P38 Q9 Q12 Q23">
-    <cfRule type="cellIs" dxfId="89" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="12" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="containsText" dxfId="88" priority="13" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(B5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="cellIs" dxfId="87" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="14" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="cellIs" dxfId="86" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="15" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="cellIs" dxfId="85" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="cellIs" dxfId="84" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="17" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="cellIs" dxfId="83" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="18" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B11">
-    <cfRule type="cellIs" dxfId="82" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="19" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="81" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="29" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="80" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="79" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="31" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="78" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="32" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="77" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="33" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12475,17 +12429,17 @@
         <v>0</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="125" t="s">
+      <c r="H3" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="117"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="123"/>
     </row>
     <row r="4" spans="2:20">
       <c r="E4" s="20"/>
@@ -12504,11 +12458,11 @@
       <c r="P4" s="34"/>
     </row>
     <row r="5" spans="2:20">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
       <c r="E5" s="20"/>
       <c r="F5" s="61" t="s">
         <v>41</v>
@@ -12529,10 +12483,10 @@
       <c r="P5" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="S5" s="131" t="s">
+      <c r="S5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="131"/>
+      <c r="T5" s="117"/>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="11" t="s">
@@ -12541,7 +12495,7 @@
       <c r="C6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="119"/>
       <c r="E6" s="20"/>
       <c r="F6" s="61" t="s">
         <v>91</v>
@@ -12573,10 +12527,10 @@
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="114"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="20"/>
       <c r="F7" s="61" t="s">
         <v>92</v>
@@ -12608,10 +12562,10 @@
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="114"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="20"/>
       <c r="F8" s="61" t="s">
         <v>93</v>
@@ -12646,10 +12600,10 @@
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="20"/>
       <c r="F9" s="61" t="s">
         <v>94</v>
@@ -12681,10 +12635,10 @@
       <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="20"/>
       <c r="F10" s="61" t="s">
         <v>95</v>
@@ -12698,11 +12652,11 @@
       <c r="I10" s="10"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="119" t="s">
+      <c r="L10" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="120"/>
-      <c r="N10" s="121"/>
+      <c r="M10" s="126"/>
+      <c r="N10" s="127"/>
       <c r="O10" s="8"/>
       <c r="P10" s="88" t="s">
         <v>9</v>
@@ -12718,10 +12672,10 @@
       <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="20"/>
       <c r="F11" s="61" t="s">
         <v>97</v>
@@ -12735,11 +12689,11 @@
       <c r="I11" s="28"/>
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
-      <c r="L11" s="122" t="s">
+      <c r="L11" s="128" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="123"/>
-      <c r="N11" s="124"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="130"/>
       <c r="O11" s="29"/>
       <c r="P11" s="91" t="s">
         <v>12</v>
@@ -12749,10 +12703,10 @@
       <c r="B12" s="11">
         <v>12</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="119"/>
       <c r="I12" s="33" t="s">
         <v>24</v>
       </c>
@@ -15711,6 +15665,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="H3:P3"/>
@@ -15718,133 +15677,128 @@
     <mergeCell ref="S5:T5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="containsText" dxfId="76" priority="1" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="cellIs" dxfId="73" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="cellIs" dxfId="72" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="cellIs" dxfId="71" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="6" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G990">
-    <cfRule type="cellIs" dxfId="70" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="7" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P11">
-    <cfRule type="cellIs" dxfId="69" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P11">
-    <cfRule type="cellIs" dxfId="68" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="9" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P11">
-    <cfRule type="cellIs" dxfId="67" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P11">
-    <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P11">
-    <cfRule type="cellIs" dxfId="65" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="containsText" dxfId="64" priority="13" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(B6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="63" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="14" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="62" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="61" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="60" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="55" priority="17" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="59" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="54" priority="18" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="58" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="19" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="57" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="29" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="56" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="30" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="55" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="31" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="54" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="32" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="53" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="33" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15888,22 +15842,22 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="2:20" ht="23.25">
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="125" t="s">
+      <c r="G3" s="123"/>
+      <c r="H3" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="122"/>
     </row>
     <row r="4" spans="2:20">
       <c r="F4" s="92" t="s">
@@ -15930,11 +15884,11 @@
       </c>
     </row>
     <row r="5" spans="2:20">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
       <c r="F5" s="61" t="s">
         <v>99</v>
       </c>
@@ -15954,10 +15908,10 @@
       <c r="P5" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="131" t="s">
+      <c r="S5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="131"/>
+      <c r="T5" s="117"/>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="11" t="s">
@@ -15966,7 +15920,7 @@
       <c r="C6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="119"/>
       <c r="F6" s="61" t="s">
         <v>100</v>
       </c>
@@ -15997,10 +15951,10 @@
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="114"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="20"/>
       <c r="F7" s="61" t="s">
         <v>101</v>
@@ -16032,10 +15986,10 @@
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="114"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="20"/>
       <c r="F8" s="61" t="s">
         <v>64</v>
@@ -16067,10 +16021,10 @@
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="20"/>
       <c r="F9" s="66" t="s">
         <v>63</v>
@@ -16102,10 +16056,10 @@
       <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="20"/>
       <c r="F10" s="61" t="s">
         <v>34</v>
@@ -16137,10 +16091,10 @@
       <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="20"/>
       <c r="F11" s="61" t="s">
         <v>103</v>
@@ -16169,10 +16123,10 @@
       <c r="B12" s="11">
         <v>12</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="20"/>
       <c r="F12" s="61" t="s">
         <v>104</v>
@@ -16321,11 +16275,11 @@
       <c r="H18" s="97">
         <v>1</v>
       </c>
-      <c r="I18" s="126" t="s">
+      <c r="I18" s="132" t="s">
         <v>108</v>
       </c>
-      <c r="J18" s="127"/>
-      <c r="K18" s="128"/>
+      <c r="J18" s="133"/>
+      <c r="K18" s="134"/>
       <c r="L18" s="28"/>
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
@@ -19296,6 +19250,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="H3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -19303,133 +19262,128 @@
     <mergeCell ref="S5:T5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="containsText" dxfId="52" priority="1" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="48" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="47" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P18 Q4 S10 Q11 Q15:Q16 Q18">
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="8" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P18 Q4 S10 Q11 Q15:Q16 Q18">
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P18 Q4 S10 Q11 Q15:Q16 Q18">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P18 Q4 S10 Q11 Q15:Q16 Q18">
-    <cfRule type="cellIs" dxfId="42" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P18 Q4 S10 Q11 Q15:Q16 Q18">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="containsText" dxfId="40" priority="13" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(B6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="14" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="38" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="37" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="36" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="35" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="34" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19446,7 +19400,7 @@
   <dimension ref="B1:T997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -19476,22 +19430,22 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="2:20" ht="23.25">
-      <c r="F3" s="130" t="s">
+      <c r="F3" s="135" t="s">
         <v>109</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="125" t="s">
+      <c r="G3" s="123"/>
+      <c r="H3" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="122"/>
     </row>
     <row r="4" spans="2:20">
       <c r="G4" s="66"/>
@@ -19507,28 +19461,34 @@
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="2:20">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="66"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="F5" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="66">
+        <v>2</v>
+      </c>
       <c r="H5" s="95">
         <v>14</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="L5" s="116"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="88"/>
-      <c r="S5" s="131" t="s">
+      <c r="P5" s="88" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="131"/>
+      <c r="T5" s="117"/>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="11" t="s">
@@ -19537,20 +19497,26 @@
       <c r="C6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="114"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="66"/>
+      <c r="D6" s="119"/>
+      <c r="F6" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="66">
+        <v>2</v>
+      </c>
       <c r="H6" s="97">
         <v>13</v>
       </c>
       <c r="I6" s="81"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="L6" s="116"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="99"/>
+      <c r="P6" s="88" t="s">
+        <v>18</v>
+      </c>
       <c r="S6" s="100" t="s">
         <v>6</v>
       </c>
@@ -19562,24 +19528,30 @@
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="114"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
+      <c r="F7" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="61">
+        <v>2</v>
+      </c>
       <c r="H7" s="95">
         <v>12</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="116"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
-      <c r="P7" s="99"/>
+      <c r="P7" s="88" t="s">
+        <v>18</v>
+      </c>
       <c r="S7" s="14" t="s">
         <v>9</v>
       </c>
@@ -19591,10 +19563,10 @@
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="114"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="20"/>
       <c r="F8" s="61" t="s">
         <v>98</v>
@@ -19605,8 +19577,8 @@
       <c r="H8" s="95">
         <v>11</v>
       </c>
-      <c r="I8" s="134"/>
-      <c r="J8" s="135"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="116"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -19626,10 +19598,10 @@
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="20"/>
       <c r="F9" s="61" t="s">
         <v>64</v>
@@ -19640,8 +19612,8 @@
       <c r="H9" s="95">
         <v>10</v>
       </c>
-      <c r="I9" s="132"/>
-      <c r="J9" s="133"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="114"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -19661,10 +19633,10 @@
       <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="20"/>
       <c r="F10" s="66" t="s">
         <v>63</v>
@@ -19696,10 +19668,10 @@
       <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="20"/>
       <c r="F11" s="61" t="s">
         <v>34</v>
@@ -19725,10 +19697,10 @@
       <c r="B12" s="11">
         <v>12</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="20"/>
       <c r="F12" s="61" t="s">
         <v>110</v>
@@ -22858,126 +22830,126 @@
     <mergeCell ref="C11:D11"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G2 G4:G997">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P18 S10 Q17:Q18">
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+  <conditionalFormatting sqref="S10 Q17:Q18 P4:P18">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P18 S10 Q17:Q18">
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+  <conditionalFormatting sqref="S10 Q17:Q18 P4:P18">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P18 S10 Q17:Q18">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+  <conditionalFormatting sqref="S10 Q17:Q18 P4:P18">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P18 S10 Q17:Q18">
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+  <conditionalFormatting sqref="S10 Q17:Q18 P4:P18">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P18 S10 Q17:Q18">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+  <conditionalFormatting sqref="S10 Q17:Q18 P4:P18">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="Nº">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Nº">
       <formula>NOT(ISERROR(SEARCH(("Nº"),(B6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="between">
       <formula>5</formula>
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B12">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="19" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="9" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="29" operator="equal">
       <formula>"ALL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="8" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="30" operator="equal">
       <formula>"TL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="31" operator="equal">
       <formula>"IC"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="6" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="32" operator="equal">
       <formula>"DL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="5" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="equal">
       <formula>"DM"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>